<commit_message>
Code before meeting with Julie Forman on 26082024
Likely unblinding tomorrow to see the PP effects.
</commit_message>
<xml_diff>
--- a/Data/easy_trial_seperate_schemes/anamnese_og_objektiv_undersøgelse_baseline_followup.mITT.data .xlsx
+++ b/Data/easy_trial_seperate_schemes/anamnese_og_objektiv_undersøgelse_baseline_followup.mITT.data .xlsx
@@ -672,7 +672,7 @@
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>tidligere_medicin_sle_001</t>
+          <t>aktuel_medicin_sle</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
@@ -792,7 +792,7 @@
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
-          <t>dosis_tnf</t>
+          <t>dosis_rtx</t>
         </is>
       </c>
       <c r="CE1" s="1" t="inlineStr">
@@ -802,12 +802,12 @@
       </c>
       <c r="CF1" s="1" t="inlineStr">
         <is>
-          <t>start_tnf</t>
+          <t>seneste_rtx</t>
         </is>
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>bemærk_tnf</t>
+          <t>bemærk_rtx</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
@@ -817,12 +817,12 @@
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>dosis_il_6</t>
+          <t>dosis_cyclo</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
-          <t>admin_il_6</t>
+          <t>admin_cyclo</t>
         </is>
       </c>
       <c r="CK1" s="1" t="inlineStr">
@@ -832,12 +832,12 @@
       </c>
       <c r="CL1" s="1" t="inlineStr">
         <is>
-          <t>slut_il_6</t>
+          <t>senest_cyclo</t>
         </is>
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>bemærk_il_6</t>
+          <t>bemærk_cyclo</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
@@ -1468,21 +1468,23 @@
       </c>
       <c r="EO2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="EP2">
         <v>10</v>
       </c>
-      <c r="EQ2">
-        <v>2</v>
+      <c r="EQ2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="ER2">
         <v>4</v>
       </c>
       <c r="ES2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET2" t="inlineStr">
@@ -1904,15 +1906,17 @@
       <c r="EP3">
         <v>10</v>
       </c>
-      <c r="EQ3">
-        <v>0</v>
+      <c r="EQ3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER3">
         <v>0</v>
       </c>
       <c r="ES3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET3" t="inlineStr">
@@ -2564,15 +2568,17 @@
       <c r="EP5">
         <v>4</v>
       </c>
-      <c r="EQ5">
-        <v>0</v>
+      <c r="EQ5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER5">
         <v>3</v>
       </c>
       <c r="ES5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="ET5" t="inlineStr">
@@ -3070,15 +3076,17 @@
       <c r="EP7">
         <v>10</v>
       </c>
-      <c r="EQ7">
-        <v>0</v>
+      <c r="EQ7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="ER7">
         <v>4</v>
       </c>
       <c r="ES7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET7" t="inlineStr">
@@ -3650,15 +3658,17 @@
       <c r="EP9">
         <v>0</v>
       </c>
-      <c r="EQ9">
-        <v>2</v>
+      <c r="EQ9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER9">
         <v>0</v>
       </c>
       <c r="ES9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="ET9" t="inlineStr">
@@ -4195,15 +4205,17 @@
       <c r="EP11">
         <v>0</v>
       </c>
-      <c r="EQ11">
-        <v>0</v>
+      <c r="EQ11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER11">
         <v>0</v>
       </c>
       <c r="ES11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET11" t="inlineStr">
@@ -4618,15 +4630,17 @@
       <c r="EP13">
         <v>0</v>
       </c>
-      <c r="EQ13">
-        <v>0</v>
+      <c r="EQ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER13">
         <v>0</v>
       </c>
       <c r="ES13" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET13" t="inlineStr">
@@ -5129,14 +5143,16 @@
       </c>
       <c r="EO15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="EP15">
         <v>0</v>
       </c>
-      <c r="EQ15">
-        <v>0</v>
+      <c r="EQ15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER15">
         <v>4</v>
@@ -5717,14 +5733,16 @@
       </c>
       <c r="EO17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="EP17">
         <v>0</v>
       </c>
-      <c r="EQ17">
-        <v>0</v>
+      <c r="EQ17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER17">
         <v>0</v>
@@ -6341,21 +6359,23 @@
       </c>
       <c r="EO19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2	3</t>
         </is>
       </c>
       <c r="EP19">
         <v>8</v>
       </c>
-      <c r="EQ19">
-        <v>2</v>
+      <c r="EQ19" t="inlineStr">
+        <is>
+          <t>1	3	4</t>
+        </is>
       </c>
       <c r="ER19">
         <v>4</v>
       </c>
       <c r="ES19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="ET19" t="inlineStr">
@@ -6678,8 +6698,10 @@
       <c r="EP20">
         <v>4</v>
       </c>
-      <c r="EQ20">
-        <v>0</v>
+      <c r="EQ20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER20">
         <v>0</v>
@@ -7237,8 +7259,10 @@
       <c r="EP22">
         <v>0</v>
       </c>
-      <c r="EQ22">
-        <v>0</v>
+      <c r="EQ22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER22">
         <v>0</v>
@@ -7878,21 +7902,23 @@
       </c>
       <c r="EO24" t="inlineStr">
         <is>
-          <t>4	4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="EP24">
         <v>10</v>
       </c>
-      <c r="EQ24">
-        <v>2</v>
+      <c r="EQ24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="ER24">
         <v>4</v>
       </c>
       <c r="ES24" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET24" t="inlineStr">
@@ -8542,8 +8568,10 @@
       <c r="EP26">
         <v>0</v>
       </c>
-      <c r="EQ26">
-        <v>0</v>
+      <c r="EQ26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER26">
         <v>0</v>
@@ -9215,15 +9243,17 @@
       <c r="EP28">
         <v>10</v>
       </c>
-      <c r="EQ28">
-        <v>2</v>
+      <c r="EQ28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="ER28">
         <v>4</v>
       </c>
       <c r="ES28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET28" t="inlineStr">
@@ -9889,21 +9919,23 @@
       </c>
       <c r="EO30" t="inlineStr">
         <is>
-          <t>3	4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="EP30">
         <v>10</v>
       </c>
-      <c r="EQ30">
-        <v>2</v>
+      <c r="EQ30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="ER30">
         <v>4</v>
       </c>
       <c r="ES30" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1	2</t>
         </is>
       </c>
       <c r="ET30" t="inlineStr">
@@ -10529,15 +10561,17 @@
       <c r="EP32">
         <v>10</v>
       </c>
-      <c r="EQ32">
-        <v>2</v>
+      <c r="EQ32" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="ER32">
         <v>4</v>
       </c>
       <c r="ES32" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1	2</t>
         </is>
       </c>
       <c r="ET32" t="inlineStr">
@@ -11160,15 +11194,17 @@
       <c r="EP34">
         <v>4</v>
       </c>
-      <c r="EQ34">
-        <v>2</v>
+      <c r="EQ34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER34">
         <v>4</v>
       </c>
       <c r="ES34" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET34" t="inlineStr">
@@ -11696,8 +11732,10 @@
       <c r="EP36">
         <v>0</v>
       </c>
-      <c r="EQ36">
-        <v>0</v>
+      <c r="EQ36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER36">
         <v>3</v>
@@ -12320,15 +12358,17 @@
       <c r="EP38">
         <v>0</v>
       </c>
-      <c r="EQ38">
-        <v>2</v>
+      <c r="EQ38" t="inlineStr">
+        <is>
+          <t>1	3	4</t>
+        </is>
       </c>
       <c r="ER38">
         <v>0</v>
       </c>
       <c r="ES38" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET38" t="inlineStr">
@@ -12979,15 +13019,17 @@
       <c r="EP40">
         <v>8</v>
       </c>
-      <c r="EQ40">
-        <v>0</v>
+      <c r="EQ40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER40">
         <v>4</v>
       </c>
       <c r="ES40" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET40" t="inlineStr">
@@ -13610,8 +13652,10 @@
       <c r="EP42">
         <v>0</v>
       </c>
-      <c r="EQ42">
-        <v>0</v>
+      <c r="EQ42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER42">
         <v>0</v>
@@ -14224,8 +14268,10 @@
       <c r="EP44">
         <v>0</v>
       </c>
-      <c r="EQ44">
-        <v>0</v>
+      <c r="EQ44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER44">
         <v>0</v>
@@ -14831,8 +14877,10 @@
       <c r="EP46">
         <v>0</v>
       </c>
-      <c r="EQ46">
-        <v>0</v>
+      <c r="EQ46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER46">
         <v>0</v>
@@ -15446,15 +15494,17 @@
       <c r="EP48">
         <v>0</v>
       </c>
-      <c r="EQ48">
-        <v>2</v>
+      <c r="EQ48" t="inlineStr">
+        <is>
+          <t>1	3	4</t>
+        </is>
       </c>
       <c r="ER48">
         <v>0</v>
       </c>
       <c r="ES48" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET48" t="inlineStr">
@@ -16002,21 +16052,23 @@
       </c>
       <c r="EO50" t="inlineStr">
         <is>
-          <t>4	4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="EP50">
         <v>4</v>
       </c>
-      <c r="EQ50">
-        <v>0</v>
+      <c r="EQ50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER50">
         <v>4</v>
       </c>
       <c r="ES50" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1	2</t>
         </is>
       </c>
       <c r="ET50" t="inlineStr">
@@ -16651,21 +16703,23 @@
       </c>
       <c r="EO52" t="inlineStr">
         <is>
-          <t>4	4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="EP52">
         <v>10</v>
       </c>
-      <c r="EQ52">
-        <v>2</v>
+      <c r="EQ52" t="inlineStr">
+        <is>
+          <t>1	3	4</t>
+        </is>
       </c>
       <c r="ER52">
         <v>4</v>
       </c>
       <c r="ES52" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET52" t="inlineStr">
@@ -17326,21 +17380,23 @@
       </c>
       <c r="EO54" t="inlineStr">
         <is>
-          <t>4	4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="EP54">
         <v>0</v>
       </c>
-      <c r="EQ54">
-        <v>2</v>
+      <c r="EQ54" t="inlineStr">
+        <is>
+          <t>1	4</t>
+        </is>
       </c>
       <c r="ER54">
         <v>4</v>
       </c>
       <c r="ES54" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET54" t="inlineStr">
@@ -18011,15 +18067,17 @@
       <c r="EP56">
         <v>0</v>
       </c>
-      <c r="EQ56">
-        <v>0</v>
+      <c r="EQ56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER56">
         <v>0</v>
       </c>
       <c r="ES56" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET56" t="inlineStr">
@@ -18589,15 +18647,17 @@
       <c r="EP58">
         <v>0</v>
       </c>
-      <c r="EQ58">
-        <v>0</v>
+      <c r="EQ58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER58">
         <v>0</v>
       </c>
       <c r="ES58" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET58" t="inlineStr">
@@ -19080,7 +19140,7 @@
       </c>
       <c r="CP60" t="inlineStr">
         <is>
-          <t>Predmisolon</t>
+          <t>Prednisolon</t>
         </is>
       </c>
       <c r="CQ60" t="inlineStr">
@@ -19208,15 +19268,17 @@
       <c r="EP60">
         <v>10</v>
       </c>
-      <c r="EQ60">
-        <v>2</v>
+      <c r="EQ60" t="inlineStr">
+        <is>
+          <t>1	4</t>
+        </is>
       </c>
       <c r="ER60">
         <v>4</v>
       </c>
       <c r="ES60" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET60" t="inlineStr">
@@ -19747,15 +19809,17 @@
       <c r="EP62">
         <v>0</v>
       </c>
-      <c r="EQ62">
-        <v>0</v>
+      <c r="EQ62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER62">
         <v>4</v>
       </c>
       <c r="ES62" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET62" t="inlineStr">
@@ -20255,15 +20319,17 @@
       <c r="EP64">
         <v>10</v>
       </c>
-      <c r="EQ64">
-        <v>0</v>
+      <c r="EQ64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER64">
         <v>4</v>
       </c>
       <c r="ES64" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET64" t="inlineStr">
@@ -20803,21 +20869,23 @@
       </c>
       <c r="EO66" t="inlineStr">
         <is>
-          <t>4	4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="EP66">
         <v>0</v>
       </c>
-      <c r="EQ66">
-        <v>0</v>
+      <c r="EQ66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER66">
         <v>3</v>
       </c>
       <c r="ES66" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="ET66" t="inlineStr">
@@ -21377,21 +21445,23 @@
       </c>
       <c r="EO68" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="EP68">
         <v>4</v>
       </c>
-      <c r="EQ68">
-        <v>2</v>
+      <c r="EQ68" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="ER68">
         <v>4</v>
       </c>
       <c r="ES68" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET68" t="inlineStr">
@@ -21932,15 +22002,17 @@
       <c r="EP70">
         <v>4</v>
       </c>
-      <c r="EQ70">
-        <v>0</v>
+      <c r="EQ70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER70">
         <v>0</v>
       </c>
       <c r="ES70" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET70" t="inlineStr">
@@ -22512,15 +22584,17 @@
       <c r="EP72">
         <v>0</v>
       </c>
-      <c r="EQ72">
-        <v>2</v>
+      <c r="EQ72" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="ER72">
         <v>0</v>
       </c>
       <c r="ES72" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="ET72" t="inlineStr">
@@ -23131,15 +23205,17 @@
       <c r="EP74">
         <v>4</v>
       </c>
-      <c r="EQ74">
-        <v>0</v>
+      <c r="EQ74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER74">
         <v>4</v>
       </c>
       <c r="ES74" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="ET74" t="inlineStr">
@@ -23747,15 +23823,17 @@
       <c r="EP76">
         <v>4</v>
       </c>
-      <c r="EQ76">
-        <v>2</v>
+      <c r="EQ76" t="inlineStr">
+        <is>
+          <t>1	3	4</t>
+        </is>
       </c>
       <c r="ER76">
         <v>4</v>
       </c>
       <c r="ES76" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET76" t="inlineStr">
@@ -24336,15 +24414,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="EQ78">
-        <v>2</v>
+      <c r="EP78">
+        <v>8</v>
+      </c>
+      <c r="EQ78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER78">
         <v>4</v>
       </c>
       <c r="ES78" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="ET78" t="inlineStr">
@@ -24871,21 +24954,23 @@
       </c>
       <c r="EO80" t="inlineStr">
         <is>
-          <t>3	4	4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="EP80">
         <v>0</v>
       </c>
-      <c r="EQ80">
-        <v>0</v>
+      <c r="EQ80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER80">
         <v>4</v>
       </c>
       <c r="ES80" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET80" t="inlineStr">
@@ -25415,8 +25500,10 @@
       <c r="EP82">
         <v>0</v>
       </c>
-      <c r="EQ82">
-        <v>0</v>
+      <c r="EQ82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER82">
         <v>3</v>
@@ -25981,15 +26068,17 @@
       <c r="EP84">
         <v>10</v>
       </c>
-      <c r="EQ84">
-        <v>0</v>
+      <c r="EQ84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER84">
         <v>0</v>
       </c>
       <c r="ES84" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET84" t="inlineStr">
@@ -26336,8 +26425,10 @@
       <c r="EP85">
         <v>0</v>
       </c>
-      <c r="EQ85">
-        <v>0</v>
+      <c r="EQ85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER85">
         <v>3</v>
@@ -26869,15 +26960,17 @@
       <c r="EP87">
         <v>10</v>
       </c>
-      <c r="EQ87">
-        <v>2</v>
+      <c r="EQ87" t="inlineStr">
+        <is>
+          <t>1	3	4</t>
+        </is>
       </c>
       <c r="ER87">
         <v>4</v>
       </c>
       <c r="ES87" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET87" t="inlineStr">
@@ -27872,8 +27965,10 @@
       <c r="EP91">
         <v>0</v>
       </c>
-      <c r="EQ91">
-        <v>0</v>
+      <c r="EQ91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER91">
         <v>3</v>
@@ -28428,15 +28523,17 @@
       <c r="EP93">
         <v>0</v>
       </c>
-      <c r="EQ93">
-        <v>2</v>
+      <c r="EQ93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="ER93">
         <v>0</v>
       </c>
       <c r="ES93" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET93" t="inlineStr">
@@ -28982,14 +29079,16 @@
       </c>
       <c r="EO95" t="inlineStr">
         <is>
-          <t>3	4	4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="EP95">
         <v>0</v>
       </c>
-      <c r="EQ95">
-        <v>2</v>
+      <c r="EQ95" t="inlineStr">
+        <is>
+          <t>1	3	4</t>
+        </is>
       </c>
       <c r="ER95">
         <v>3</v>
@@ -29601,8 +29700,10 @@
       <c r="EP97">
         <v>10</v>
       </c>
-      <c r="EQ97">
-        <v>0</v>
+      <c r="EQ97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER97">
         <v>3</v>
@@ -30269,15 +30370,17 @@
       <c r="EP99">
         <v>4</v>
       </c>
-      <c r="EQ99">
-        <v>0</v>
+      <c r="EQ99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER99">
         <v>0</v>
       </c>
       <c r="ES99" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="ET99" t="inlineStr">
@@ -30645,15 +30748,17 @@
       <c r="EP100">
         <v>4</v>
       </c>
-      <c r="EQ100">
-        <v>0</v>
+      <c r="EQ100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="ER100">
         <v>0</v>
       </c>
       <c r="ES100" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="ET100" t="inlineStr">
@@ -31286,15 +31391,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="EQ102">
-        <v>2</v>
+      <c r="EP102">
+        <v>10</v>
+      </c>
+      <c r="EQ102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="ER102">
         <v>4</v>
       </c>
       <c r="ES102" t="inlineStr">
         <is>
-          <t>6	6</t>
+          <t>1	2</t>
         </is>
       </c>
       <c r="ET102" t="inlineStr">

</xml_diff>